<commit_message>
Update Initial issue with label Testcase
</commit_message>
<xml_diff>
--- a/Testcase Generate from Gitlab/input/config.xlsx
+++ b/Testcase Generate from Gitlab/input/config.xlsx
@@ -13,40 +13,71 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Note</t>
   </si>
   <si>
-    <t>v_Project</t>
-  </si>
-  <si>
-    <t>v_GitlabProjectUrl</t>
-  </si>
-  <si>
-    <t>https://git.iptp.net/erp/erp-server/-/issues</t>
-  </si>
-  <si>
     <t>erp-server</t>
+  </si>
+  <si>
+    <t>https://git.iptp.net/erp/erp-web/-/issues</t>
+  </si>
+  <si>
+    <t>erp-web</t>
+  </si>
+  <si>
+    <t>ERP web project</t>
+  </si>
+  <si>
+    <t>URL to Erp Web Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.iptp.net/erp/erp-server/-/issues </t>
+  </si>
+  <si>
+    <t>https://git.iptp.net/xm/xm-web/-/issues</t>
+  </si>
+  <si>
+    <t>https://git.iptp.net/andre/xm-api/-/issues</t>
+  </si>
+  <si>
+    <t>xm-api</t>
+  </si>
+  <si>
+    <t>xm-web</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Erp Server Project</t>
+  </si>
+  <si>
+    <t>Erp Web Project</t>
+  </si>
+  <si>
+    <t>XM Web Project</t>
+  </si>
+  <si>
+    <t>XM API Project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +89,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,10 +119,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -91,8 +131,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -395,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,33 +454,79 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>